<commit_message>
chore: update economic calendar data (2026-01-11..2026-01-24)
</commit_message>
<xml_diff>
--- a/data/Economic_Calendar/2026/2026_calendar.xlsx
+++ b/data/Economic_Calendar/2026/2026_calendar.xlsx
@@ -52260,7 +52260,11 @@
           <t>GDP (YoY)  (Q4)</t>
         </is>
       </c>
-      <c r="G1230" s="5" t="inlineStr"/>
+      <c r="G1230" s="5" t="inlineStr">
+        <is>
+          <t>5.7%</t>
+        </is>
+      </c>
       <c r="H1230" s="5" t="inlineStr"/>
       <c r="I1230" s="5" t="inlineStr">
         <is>

</xml_diff>